<commit_message>
Completed initial MCU Pinouts
CubeMX Project completed with all pins selected
Completed list of MCU resources
Generated CubeMX Pinout report
</commit_message>
<xml_diff>
--- a/System Design/Microcontroller Resources List.xlsx
+++ b/System Design/Microcontroller Resources List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Dropbox\Senior Design Team Folder\System Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HandGitRepo\ProstheticHand\System Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="224">
   <si>
     <t>Number</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Timer &amp; Channel</t>
-  </si>
-  <si>
     <t>TIM1 CH1</t>
   </si>
   <si>
-    <t>TIM2 CH2</t>
-  </si>
-  <si>
     <t>Ext Interrupt</t>
   </si>
   <si>
@@ -197,27 +191,12 @@
     <t>TIM1 CH3</t>
   </si>
   <si>
-    <t>TIM2 CH3</t>
-  </si>
-  <si>
     <t>TIM1 CH4</t>
   </si>
   <si>
     <t>TIM2 CH4</t>
   </si>
   <si>
-    <t>TIM8 CH1</t>
-  </si>
-  <si>
-    <t>TIM8 CH2</t>
-  </si>
-  <si>
-    <t>TIM5 CH1</t>
-  </si>
-  <si>
-    <t>TIM5 CH2</t>
-  </si>
-  <si>
     <t>Pointer Limit Switch</t>
   </si>
   <si>
@@ -245,33 +224,21 @@
     <t>EMG Signal (Processed)</t>
   </si>
   <si>
-    <t>Mode 1 Activation LED</t>
-  </si>
-  <si>
     <t>Mode 1 Button (Grab)</t>
   </si>
   <si>
     <t xml:space="preserve">Mode 2 Button (Pinch) </t>
   </si>
   <si>
-    <t>Mode 2 Activation LED</t>
-  </si>
-  <si>
     <t>Mode 3 Button (Point)</t>
   </si>
   <si>
-    <t>Mode 3 Activation LED</t>
-  </si>
-  <si>
     <t>Mode 4 Button (Handshake)</t>
   </si>
   <si>
     <t>Manual EMG Override Button</t>
   </si>
   <si>
-    <t>Master Reset Button</t>
-  </si>
-  <si>
     <t>User Input/Output</t>
   </si>
   <si>
@@ -287,15 +254,9 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Power Good LED (Direct 3.3V conn)</t>
-  </si>
-  <si>
     <t>General MCU I/O</t>
   </si>
   <si>
-    <t>Motor Enable</t>
-  </si>
-  <si>
     <t>UART</t>
   </si>
   <si>
@@ -329,15 +290,6 @@
     <t>TDI</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>UART Interrupt</t>
-  </si>
-  <si>
-    <t>Mode 4 Activation LED</t>
-  </si>
-  <si>
     <t>MCU Port/Num</t>
   </si>
   <si>
@@ -365,9 +317,6 @@
     <t>PE0</t>
   </si>
   <si>
-    <t>Polling now, need to figure out interrupts</t>
-  </si>
-  <si>
     <t>User Defined Button (Wakeup)</t>
   </si>
   <si>
@@ -398,9 +347,6 @@
     <t>PE14</t>
   </si>
   <si>
-    <t>TIM2 CH1***Cant use</t>
-  </si>
-  <si>
     <t>PA1</t>
   </si>
   <si>
@@ -408,6 +354,348 @@
   </si>
   <si>
     <t>PA3</t>
+  </si>
+  <si>
+    <t>TIM2 CH1</t>
+  </si>
+  <si>
+    <t>TIM3 CH1</t>
+  </si>
+  <si>
+    <t>TIM3 CH2</t>
+  </si>
+  <si>
+    <t>TIM3 CH3</t>
+  </si>
+  <si>
+    <t>TIM3 CH4</t>
+  </si>
+  <si>
+    <t>Peripheral</t>
+  </si>
+  <si>
+    <t>USART1</t>
+  </si>
+  <si>
+    <t>USART2</t>
+  </si>
+  <si>
+    <t>SYS_JTMS</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>PE8</t>
+  </si>
+  <si>
+    <t>PE10</t>
+  </si>
+  <si>
+    <t>PE12</t>
+  </si>
+  <si>
+    <t>PE15</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PB14</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>PD8</t>
+  </si>
+  <si>
+    <t>PD9</t>
+  </si>
+  <si>
+    <t>PD0</t>
+  </si>
+  <si>
+    <t>PD10</t>
+  </si>
+  <si>
+    <t>PD11</t>
+  </si>
+  <si>
+    <t>PD13</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
+    <t>PD14</t>
+  </si>
+  <si>
+    <t>PD15</t>
+  </si>
+  <si>
+    <t>PA8</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>PD7</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PE6</t>
+  </si>
+  <si>
+    <t>TIM4 CH1</t>
+  </si>
+  <si>
+    <t>TIM4 CH2</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>ADC1 IN2</t>
+  </si>
+  <si>
+    <t>ADC1 IN3</t>
+  </si>
+  <si>
+    <t>ADC1 IN4</t>
+  </si>
+  <si>
+    <t>ADC1 IN8</t>
+  </si>
+  <si>
+    <t>ADC1 IN9</t>
+  </si>
+  <si>
+    <t>ADC1 IN7</t>
+  </si>
+  <si>
+    <t>ADC1 IN10</t>
+  </si>
+  <si>
+    <t>ADC1 IN11</t>
+  </si>
+  <si>
+    <t>ADC1 IN12</t>
+  </si>
+  <si>
+    <t>ADC1 IN13</t>
+  </si>
+  <si>
+    <t>ADC1 IN1</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>ADC1 IN6</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>PC10</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>User Defined Button</t>
+  </si>
+  <si>
+    <t>Motor Driver Enable</t>
+  </si>
+  <si>
+    <t>Mode 1 Activation LED (Grab)</t>
+  </si>
+  <si>
+    <t>Mode 2 Activation LED (Pinch)</t>
+  </si>
+  <si>
+    <t>Mode 3 Activation LED (Point)</t>
+  </si>
+  <si>
+    <t>Mode 4 Activation LED (Handshake)</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>VSSA</t>
+  </si>
+  <si>
+    <t>VCAP1</t>
+  </si>
+  <si>
+    <t>VCAP2</t>
+  </si>
+  <si>
+    <t>VBAT</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>VDDA</t>
+  </si>
+  <si>
+    <t>BOOT0</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>PB2</t>
+  </si>
+  <si>
+    <t>PE7</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>Clock Inputs</t>
+  </si>
+  <si>
+    <t>High Speed Oscillator IN</t>
+  </si>
+  <si>
+    <t>High Speed Oscillator OUT</t>
+  </si>
+  <si>
+    <t>Low Speed Oscillator IN</t>
+  </si>
+  <si>
+    <t>Low Speed Oscillator OUT</t>
+  </si>
+  <si>
+    <t>Indicates External Interrupt</t>
+  </si>
+  <si>
+    <t>VREF</t>
+  </si>
+  <si>
+    <t>Mid circuit connection</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>BOOT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timers 1 and 4: PWM </t>
+  </si>
+  <si>
+    <t>Timers 2 and 3: Input Capture</t>
+  </si>
+  <si>
+    <t>EXTI pin # must not conflict (ie. Can't have both PB5 and PE5)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +728,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,14 +763,91 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -504,6 +869,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A1:I101"/>
+  <sortState ref="A2:I101">
+    <sortCondition ref="A1:A101"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Number" dataDxfId="8"/>
+    <tableColumn id="2" name="Group" dataDxfId="7"/>
+    <tableColumn id="3" name="Name/Connection" dataDxfId="6"/>
+    <tableColumn id="4" name="Input/Output" dataDxfId="5"/>
+    <tableColumn id="5" name="Analog/Digital" dataDxfId="4"/>
+    <tableColumn id="6" name="Peripheral" dataDxfId="3"/>
+    <tableColumn id="7" name="Ext Interrupt" dataDxfId="2"/>
+    <tableColumn id="8" name="MCU Port/Num" dataDxfId="1"/>
+    <tableColumn id="9" name="MCU Physical Pin" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,28 +1189,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="19.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="20.125" customWidth="1"/>
-    <col min="7" max="7" width="17.125" customWidth="1"/>
-    <col min="8" max="8" width="17.75" customWidth="1"/>
-    <col min="9" max="9" width="19.875" customWidth="1"/>
-    <col min="10" max="10" width="46.875" customWidth="1"/>
+    <col min="3" max="3" width="44.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="21.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="50.125" customWidth="1"/>
+    <col min="11" max="11" width="46.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -841,26 +1227,26 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -870,20 +1256,22 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="I2" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -891,250 +1279,341 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="1">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>67</v>
+      <c r="C6" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="1">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="3">
+        <v>60</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -1143,11 +1622,11 @@
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I16" s="1">
         <v>40</v>
@@ -1157,8 +1636,8 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -1166,120 +1645,148 @@
       <c r="E17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="I17" s="1">
-        <v>98</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I18" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="I18" s="1">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>25</v>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="1">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>64</v>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I20" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>26</v>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>27</v>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I22" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -1288,20 +1795,22 @@
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="I23" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -1309,116 +1818,148 @@
       <c r="E24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="1">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>31</v>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I25" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="I25" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>32</v>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26" s="1">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>68</v>
+      <c r="C27" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="1">
+        <v>51</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>33</v>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I28" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I29" s="1">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
@@ -1427,20 +1968,22 @@
         <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I30" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="I30" s="1">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>37</v>
+      <c r="C31" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
@@ -1448,116 +1991,148 @@
       <c r="E31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" s="1">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>38</v>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>175</v>
+      </c>
+      <c r="I32" s="1">
+        <v>65</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>39</v>
+      <c r="C33" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>69</v>
+      <c r="C34" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I34" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>40</v>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I35" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>41</v>
+      <c r="C36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
@@ -1566,18 +2141,22 @@
         <v>3</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>44</v>
+      <c r="C38" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -1585,155 +2164,201 @@
       <c r="E38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I38" s="1">
+        <v>55</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>45</v>
+      <c r="C39" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I39" s="1">
+        <v>66</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>46</v>
+      <c r="C40" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I40" s="1">
+        <v>56</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>70</v>
+      <c r="C41" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I41" s="1">
+        <v>57</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>47</v>
+      <c r="C42" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I42" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>48</v>
+      <c r="C43" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I43" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I44" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I45" s="1">
+        <v>58</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>73</v>
+      <c r="C46" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
@@ -1741,37 +2366,49 @@
       <c r="E46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I46" s="1">
+        <v>59</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>75</v>
+      <c r="C47" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" s="1">
+        <v>88</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>76</v>
+      <c r="C48" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>
@@ -1779,37 +2416,49 @@
       <c r="E48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I48" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>77</v>
+      <c r="C49" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I49" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>78</v>
+      <c r="C50" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
@@ -1817,37 +2466,49 @@
       <c r="E50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I50" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>79</v>
+      <c r="C51" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I51" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>103</v>
+      <c r="C52" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>9</v>
@@ -1855,79 +2516,101 @@
       <c r="E52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>80</v>
+      <c r="C53" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G53" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I53" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>114</v>
+      <c r="C54" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I54" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>81</v>
+      <c r="C55" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>83</v>
+      <c r="C56" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>9</v>
@@ -1935,17 +2618,23 @@
       <c r="E56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F56" s="1"/>
+      <c r="F56" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H56" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>84</v>
+      <c r="C57" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
@@ -1953,17 +2642,23 @@
       <c r="E57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I57" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>85</v>
+      <c r="C58" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>9</v>
@@ -1971,116 +2666,104 @@
       <c r="E58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I58" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>87</v>
+      <c r="B59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I59" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I60" s="1">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C61" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C62" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="I62" s="1">
-        <v>69</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>93</v>
+      <c r="B63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>9</v>
@@ -2088,160 +2771,735 @@
       <c r="E63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="I63" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>94</v>
+      <c r="C64" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="F64" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="I64" s="1">
-        <v>87</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>96</v>
+      <c r="C65" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="F65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I65" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="I65" s="1">
+        <v>86</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
+      <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I66" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I66" s="3">
+        <v>87</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>98</v>
+      <c r="B67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="F67" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I67" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="I67" s="1">
+        <v>89</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>99</v>
+      <c r="C68" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G68" s="1"/>
       <c r="H68" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I68" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="I68" s="1">
+        <v>90</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I69" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="I70" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>118</v>
+      <c r="I71" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3"/>
+      <c r="C86" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I88" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I89" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I90" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I91" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I92" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I93" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I94" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I95" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I97" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H69">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="H2:H59">
+    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60:H101">
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I101">
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>